<commit_message>
Refactor process-id and timestamp, Update Process and list
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">process-id</t>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,10 +149,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -335,17 +334,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -366,8 +367,28 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>